<commit_message>
new data sheet added
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uhche\Documents\Industrial Training\TestMVC\HelloSpringMVC - Copy - Copy (2)\src\main\webapp\WEB-INF\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uhche\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,33 +19,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>alice</t>
-  </si>
-  <si>
-    <t>bob</t>
-  </si>
-  <si>
-    <t>paris</t>
-  </si>
-  <si>
-    <t>london</t>
-  </si>
-  <si>
-    <t>new york</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>EMPLOYEE_ID</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>john.doe@email.com</t>
+  </si>
+  <si>
+    <t>jane.smith@email.com</t>
+  </si>
+  <si>
+    <t>mike.johnson@email.com</t>
+  </si>
+  <si>
+    <t>emily.white@email.com</t>
+  </si>
+  <si>
+    <t>david.brown@email.com</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Norma</t>
+  </si>
+  <si>
+    <t>Fisher</t>
   </si>
 </sst>
 </file>
@@ -413,62 +446,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>2</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>75000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>85000.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>62000.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>92000</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>35</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>70000.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>